<commit_message>
CHanged Excel reading techiique and addded data in excel
</commit_message>
<xml_diff>
--- a/Excel/login.xlsx
+++ b/Excel/login.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E280A9A9-CE20-485B-8A80-6D8B81ECD61E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DED3349-4812-4233-A93E-223F41ABB169}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
   <si>
     <t>username</t>
   </si>
@@ -44,9 +44,6 @@
     <t>test@1234</t>
   </si>
   <si>
-    <t>kaushik.aryaan@gmail</t>
-  </si>
-  <si>
     <t>Testing Done</t>
   </si>
   <si>
@@ -54,6 +51,18 @@
   </si>
   <si>
     <t>Send mail for testing</t>
+  </si>
+  <si>
+    <t>kaushik.aryaan@gmail.com</t>
+  </si>
+  <si>
+    <t>Development Done</t>
+  </si>
+  <si>
+    <t>Send mail for development</t>
+  </si>
+  <si>
+    <t>Save mail for development</t>
   </si>
 </sst>
 </file>
@@ -400,17 +409,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -440,13 +449,30 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
       <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -454,6 +480,9 @@
     <hyperlink ref="A2" r:id="rId1" display="selenium.testmay@2017" xr:uid="{78999371-0298-4622-8814-AB1901E4EE62}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{7BDE0E55-551C-43C2-8FB1-EC23484A00A1}"/>
     <hyperlink ref="C2" r:id="rId3" xr:uid="{164067CD-8FC7-4BF6-AADA-201542D3289A}"/>
+    <hyperlink ref="A3" r:id="rId4" display="selenium.testmay@2017" xr:uid="{43D81437-F6B3-4E14-9460-A16DC95CDDA8}"/>
+    <hyperlink ref="B3" r:id="rId5" xr:uid="{431A3A8A-6281-46D4-84CE-14A7C3EF2049}"/>
+    <hyperlink ref="C3" r:id="rId6" xr:uid="{F7BF6EDA-3850-47E7-914E-DC434C989619}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -461,16 +490,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3274103E-D20E-4225-8920-DD32F809CEAA}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -499,13 +530,30 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -513,6 +561,9 @@
     <hyperlink ref="A2" r:id="rId1" display="selenium.testmay@2017" xr:uid="{F71F0B25-28F5-45D4-829A-66C7D83A50DE}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{D71F4510-8CA8-4A04-A0F3-D1D2DA3AB708}"/>
     <hyperlink ref="C2" r:id="rId3" xr:uid="{C55A322F-D7A5-4F80-87A8-F6DDE16E7188}"/>
+    <hyperlink ref="A3" r:id="rId4" display="selenium.testmay@2017" xr:uid="{DF64FD45-4E0D-4829-98F2-B004AAC5F34F}"/>
+    <hyperlink ref="B3" r:id="rId5" xr:uid="{D462D3EB-045F-49AF-BB66-5CD3EE160571}"/>
+    <hyperlink ref="C3" r:id="rId6" xr:uid="{35B22632-3381-4822-8B64-4D702EECC5EF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>